<commit_message>
fix grouping example's bug
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/grouping.xlsx
+++ b/src/main/webapp/WEB-INF/books/grouping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/DOC/zssessentials/src/main/webapp/WEB-INF/books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1CF8CE-FFC5-5048-BFDD-53C9DE6A710D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F2AA2C-0699-CC44-A575-A7B58BFA4B8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36480" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{97AE6FF2-4CE4-E244-A363-2E60BB09F429}"/>
   </bookViews>
@@ -148,10 +148,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,256 +470,261 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD1C28F-C4E6-654C-8FEB-B5E462484FF8}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>95</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>1.99</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>189.05</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>50</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>19.989999999999998</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>999.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>36</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>4.99</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>179.64</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>27</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>19.989999999999998</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>539.73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>60</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>4.99</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>299.39999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>75</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>1.99</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>149.25</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>90</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>4.99</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>449.1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>32</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>1.99</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>63.68</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>